<commit_message>
fixing gender factor and starting to build needed tables
</commit_message>
<xml_diff>
--- a/age_est_data.xlsx
+++ b/age_est_data.xlsx
@@ -406,20 +406,20 @@
         </is>
       </c>
       <c r="B2">
-        <v>-2.192295931489879</v>
+        <v>-2.203792413187655</v>
       </c>
       <c r="C2">
-        <v>0.2629540384930116</v>
+        <v>0.2628864373562907</v>
       </c>
       <c r="D2">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E2">
-        <v>-8.337182969517853</v>
+        <v>-8.383058614016093</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.6522e-12</t>
+          <t>1.6358e-12</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -440,20 +440,20 @@
         </is>
       </c>
       <c r="B3">
-        <v>-3.235569149415106</v>
+        <v>-3.227907737330011</v>
       </c>
       <c r="C3">
-        <v>0.6358794833758414</v>
+        <v>0.6360182614789721</v>
       </c>
       <c r="D3">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E3">
-        <v>-5.088337073304657</v>
+        <v>-5.075180907265084</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1.2029e-06</t>
+          <t>1.2876e-06</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -474,20 +474,20 @@
         </is>
       </c>
       <c r="B4">
-        <v>-1.043273217925227</v>
+        <v>-1.024115324142357</v>
       </c>
       <c r="C4">
-        <v>0.6381667730997418</v>
+        <v>0.6381762280328127</v>
       </c>
       <c r="D4">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E4">
-        <v>-1.634797143790139</v>
+        <v>-1.604753168727714</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2.3128e-01</t>
+          <t>2.4387e-01</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -508,20 +508,20 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.6409839125594852</v>
+        <v>0.6508104198391331</v>
       </c>
       <c r="C5">
-        <v>0.4635795413300218</v>
+        <v>0.4632629851360087</v>
       </c>
       <c r="D5">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E5">
-        <v>1.382683780048804</v>
+        <v>1.404840103182564</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>3.5021e-01</t>
+          <t>3.3859e-01</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -542,20 +542,20 @@
         </is>
       </c>
       <c r="B6">
-        <v>2.758364562264252</v>
+        <v>2.751816043890911</v>
       </c>
       <c r="C6">
-        <v>1.121035147183632</v>
+        <v>1.120802280166442</v>
       </c>
       <c r="D6">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E6">
-        <v>2.460551365578564</v>
+        <v>2.455219883637513</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3.7175e-02</t>
+          <t>3.7701e-02</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -576,20 +576,20 @@
         </is>
       </c>
       <c r="B7">
-        <v>2.117380649704767</v>
+        <v>2.101005624051778</v>
       </c>
       <c r="C7">
-        <v>1.125067565651785</v>
+        <v>1.124605085809858</v>
       </c>
       <c r="D7">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E7">
-        <v>1.882003103056398</v>
+        <v>1.868216363736954</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1.4420e-01</t>
+          <t>1.4830e-01</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -610,20 +610,20 @@
         </is>
       </c>
       <c r="B8">
-        <v>-7.656954241804407</v>
+        <v>-7.709052136306413</v>
       </c>
       <c r="C8">
-        <v>0.6421782267149019</v>
+        <v>0.6428856402652804</v>
       </c>
       <c r="D8">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E8">
-        <v>-11.92340992464659</v>
+        <v>-11.99132731153452</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1.6200e-12</t>
+          <t>1.6044e-12</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -644,20 +644,20 @@
         </is>
       </c>
       <c r="B9">
-        <v>-10.22532387500486</v>
+        <v>-10.19060512808391</v>
       </c>
       <c r="C9">
-        <v>1.552925223658576</v>
+        <v>1.555375056101331</v>
       </c>
       <c r="D9">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E9">
-        <v>-6.584556499710116</v>
+        <v>-6.551863544492899</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1.8448e-10</t>
+          <t>2.2804e-10</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -678,20 +678,20 @@
         </is>
       </c>
       <c r="B10">
-        <v>-2.568369633200452</v>
+        <v>-2.481552991777493</v>
       </c>
       <c r="C10">
-        <v>1.558511171937961</v>
+        <v>1.560652337514508</v>
       </c>
       <c r="D10">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E10">
-        <v>-1.647963568978952</v>
+        <v>-1.590074183805477</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2.2590e-01</t>
+          <t>2.5018e-01</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -712,20 +712,20 @@
         </is>
       </c>
       <c r="B11">
-        <v>-0.9455592738036119</v>
+        <v>-0.9448593487129923</v>
       </c>
       <c r="C11">
-        <v>0.1186622223870234</v>
+        <v>0.1185668666661877</v>
       </c>
       <c r="D11">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E11">
-        <v>-7.968494561981304</v>
+        <v>-7.968999900901005</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1.6660e-12</t>
+          <t>1.6505e-12</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -746,20 +746,20 @@
         </is>
       </c>
       <c r="B12">
-        <v>-1.009687577843683</v>
+        <v>-1.010154017463127</v>
       </c>
       <c r="C12">
-        <v>0.2869508036466036</v>
+        <v>0.2868565345721258</v>
       </c>
       <c r="D12">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E12">
-        <v>-3.518678341417617</v>
+        <v>-3.521460715440454</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>1.2938e-03</t>
+          <t>1.2805e-03</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -780,20 +780,20 @@
         </is>
       </c>
       <c r="B13">
-        <v>-0.06412830404007142</v>
+        <v>-0.06529466875013512</v>
       </c>
       <c r="C13">
-        <v>0.2879829797768372</v>
+        <v>0.2878298192163714</v>
       </c>
       <c r="D13">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E13">
-        <v>-0.2226808823554972</v>
+        <v>-0.2268516477128831</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>9.7303e-01</t>
+          <t>9.7203e-01</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -814,20 +814,20 @@
         </is>
       </c>
       <c r="B14">
-        <v>-0.599900667348384</v>
+        <v>-0.5889609891895577</v>
       </c>
       <c r="C14">
-        <v>0.1916404641858987</v>
+        <v>0.1916663415973831</v>
       </c>
       <c r="D14">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E14">
-        <v>-3.130344470291289</v>
+        <v>-3.072845155185031</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>5.0497e-03</t>
+          <t>6.1003e-03</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -848,20 +848,20 @@
         </is>
       </c>
       <c r="B15">
-        <v>-0.7176982797026275</v>
+        <v>-0.7249886303209311</v>
       </c>
       <c r="C15">
-        <v>0.4634279057238146</v>
+        <v>0.4637108501781952</v>
       </c>
       <c r="D15">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E15">
-        <v>-1.548672988480647</v>
+        <v>-1.56344978782</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2.6854e-01</t>
+          <t>2.6189e-01</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -882,20 +882,20 @@
         </is>
       </c>
       <c r="B16">
-        <v>-0.1177976123542435</v>
+        <v>-0.1360276411313733</v>
       </c>
       <c r="C16">
-        <v>0.4650948786553886</v>
+        <v>0.4652841894452324</v>
       </c>
       <c r="D16">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E16">
-        <v>-0.2532765200399582</v>
+        <v>-0.2923538865431078</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>9.6526e-01</t>
+          <t>9.5398e-01</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -916,20 +916,20 @@
         </is>
       </c>
       <c r="B17">
-        <v>-1.23786301787999</v>
+        <v>-1.250862134081518</v>
       </c>
       <c r="C17">
-        <v>0.4176409885940505</v>
+        <v>0.4174189830227573</v>
       </c>
       <c r="D17">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E17">
-        <v>-2.96394044570946</v>
+        <v>-2.996658477348939</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>8.6479e-03</t>
+          <t>7.7968e-03</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -950,20 +950,20 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.7331264677800873</v>
+        <v>0.7417892559774648</v>
       </c>
       <c r="C18">
-        <v>1.009945835347261</v>
+        <v>1.009888903209718</v>
       </c>
       <c r="D18">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E18">
-        <v>0.7259067190746998</v>
+        <v>0.7345256033805746</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>7.4815e-01</t>
+          <t>7.4299e-01</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -984,20 +984,20 @@
         </is>
       </c>
       <c r="B19">
-        <v>1.970989485660077</v>
+        <v>1.992651390058983</v>
       </c>
       <c r="C19">
-        <v>1.013578660106164</v>
+        <v>1.013315387334802</v>
       </c>
       <c r="D19">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E19">
-        <v>1.944584631895893</v>
+        <v>1.966467118692441</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>1.2664e-01</t>
+          <t>1.2090e-01</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1018,20 +1018,20 @@
         </is>
       </c>
       <c r="B20">
-        <v>-6.449964297954659</v>
+        <v>-6.482947122466972</v>
       </c>
       <c r="C20">
-        <v>0.555252154157346</v>
+        <v>0.5553707430451689</v>
       </c>
       <c r="D20">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E20">
-        <v>-11.61627964819545</v>
+        <v>-11.67318805257933</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>1.6203e-12</t>
+          <t>1.6046e-12</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1052,20 +1052,20 @@
         </is>
       </c>
       <c r="B21">
-        <v>-7.988126711258818</v>
+        <v>-7.966146507491916</v>
       </c>
       <c r="C21">
-        <v>1.34271926361108</v>
+        <v>1.343644571473823</v>
       </c>
       <c r="D21">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E21">
-        <v>-5.94921583963555</v>
+        <v>-5.928760236610767</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>9.8249e-09</t>
+          <t>1.1100e-08</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1086,20 +1086,20 @@
         </is>
       </c>
       <c r="B22">
-        <v>-1.53816241330416</v>
+        <v>-1.483199385024944</v>
       </c>
       <c r="C22">
-        <v>1.347549090730892</v>
+        <v>1.34820346580297</v>
       </c>
       <c r="D22">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E22">
-        <v>-1.141451857957829</v>
+        <v>-1.10013022711047</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>4.8866e-01</t>
+          <t>5.1411e-01</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1120,20 +1120,20 @@
         </is>
       </c>
       <c r="B23">
-        <v>-1.542832824994379</v>
+        <v>-1.563237305416217</v>
       </c>
       <c r="C23">
-        <v>0.5893249895783741</v>
+        <v>0.5890511945642841</v>
       </c>
       <c r="D23">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E23">
-        <v>-2.617966066733708</v>
+        <v>-2.653822485790101</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2.4219e-02</t>
+          <t>2.1890e-02</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1154,20 +1154,20 @@
         </is>
       </c>
       <c r="B24">
-        <v>-5.653200786492048</v>
+        <v>-5.639602962653083</v>
       </c>
       <c r="C24">
-        <v>1.425114716097158</v>
+        <v>1.425129879108701</v>
       </c>
       <c r="D24">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E24">
-        <v>-3.966839106099468</v>
+        <v>-3.957255437083517</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2.2393e-04</t>
+          <t>2.3296e-04</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1188,20 +1188,20 @@
         </is>
       </c>
       <c r="B25">
-        <v>-4.110367961497669</v>
+        <v>-4.076365657236867</v>
       </c>
       <c r="C25">
-        <v>1.430240923705246</v>
+        <v>1.429965247525395</v>
       </c>
       <c r="D25">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E25">
-        <v>-2.873899000770559</v>
+        <v>-2.85067463303123</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>1.1438e-02</t>
+          <t>1.2277e-02</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1222,20 +1222,20 @@
         </is>
       </c>
       <c r="B26">
-        <v>-0.8087087729888879</v>
+        <v>-0.8181144745052047</v>
       </c>
       <c r="C26">
-        <v>0.2919906234240657</v>
+        <v>0.2918412652427201</v>
       </c>
       <c r="D26">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E26">
-        <v>-2.76963952987757</v>
+        <v>-2.80328579930186</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>1.5651e-02</t>
+          <t>1.4161e-02</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1256,20 +1256,20 @@
         </is>
       </c>
       <c r="B27">
-        <v>-2.026041405947686</v>
+        <v>-2.019773318270061</v>
       </c>
       <c r="C27">
-        <v>0.7060961977901671</v>
+        <v>0.7060705604067814</v>
       </c>
       <c r="D27">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E27">
-        <v>-2.86935606265617</v>
+        <v>-2.860582824904113</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>1.1598e-02</t>
+          <t>1.1912e-02</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1290,20 +1290,20 @@
         </is>
       </c>
       <c r="B28">
-        <v>-1.217332632958798</v>
+        <v>-1.201658843764856</v>
       </c>
       <c r="C28">
-        <v>0.7086360604835134</v>
+        <v>0.7084662096299126</v>
       </c>
       <c r="D28">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E28">
-        <v>-1.717853071332827</v>
+        <v>-1.696141364868448</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>1.9876e-01</t>
+          <t>2.0694e-01</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">

</xml_diff>

<commit_message>
changing white to White
</commit_message>
<xml_diff>
--- a/age_est_data.xlsx
+++ b/age_est_data.xlsx
@@ -406,16 +406,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>-2.203792413187655</v>
+        <v>-2.204</v>
       </c>
       <c r="C2">
-        <v>0.2628864373562907</v>
+        <v>0.263</v>
       </c>
       <c r="D2">
         <v>1669</v>
       </c>
       <c r="E2">
-        <v>-8.383058614016093</v>
+        <v>-8.382999999999999</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -440,16 +440,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>-3.227907737330011</v>
+        <v>-3.228</v>
       </c>
       <c r="C3">
-        <v>0.6360182614789721</v>
+        <v>0.636</v>
       </c>
       <c r="D3">
         <v>1669</v>
       </c>
       <c r="E3">
-        <v>-5.075180907265084</v>
+        <v>-5.075</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -474,16 +474,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>-1.024115324142357</v>
+        <v>-1.024</v>
       </c>
       <c r="C4">
-        <v>0.6381762280328127</v>
+        <v>0.638</v>
       </c>
       <c r="D4">
         <v>1669</v>
       </c>
       <c r="E4">
-        <v>-1.604753168727714</v>
+        <v>-1.605</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -508,16 +508,16 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.6508104198391331</v>
+        <v>0.651</v>
       </c>
       <c r="C5">
-        <v>0.4632629851360087</v>
+        <v>0.463</v>
       </c>
       <c r="D5">
         <v>1669</v>
       </c>
       <c r="E5">
-        <v>1.404840103182564</v>
+        <v>1.405</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -542,16 +542,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>2.751816043890911</v>
+        <v>2.752</v>
       </c>
       <c r="C6">
-        <v>1.120802280166442</v>
+        <v>1.121</v>
       </c>
       <c r="D6">
         <v>1669</v>
       </c>
       <c r="E6">
-        <v>2.455219883637513</v>
+        <v>2.455</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -576,16 +576,16 @@
         </is>
       </c>
       <c r="B7">
-        <v>2.101005624051778</v>
+        <v>2.101</v>
       </c>
       <c r="C7">
-        <v>1.124605085809858</v>
+        <v>1.125</v>
       </c>
       <c r="D7">
         <v>1669</v>
       </c>
       <c r="E7">
-        <v>1.868216363736954</v>
+        <v>1.868</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -610,16 +610,16 @@
         </is>
       </c>
       <c r="B8">
-        <v>-7.709052136306413</v>
+        <v>-7.709</v>
       </c>
       <c r="C8">
-        <v>0.6428856402652804</v>
+        <v>0.643</v>
       </c>
       <c r="D8">
         <v>1669</v>
       </c>
       <c r="E8">
-        <v>-11.99132731153452</v>
+        <v>-11.991</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -644,16 +644,16 @@
         </is>
       </c>
       <c r="B9">
-        <v>-10.19060512808391</v>
+        <v>-10.191</v>
       </c>
       <c r="C9">
-        <v>1.555375056101331</v>
+        <v>1.555</v>
       </c>
       <c r="D9">
         <v>1669</v>
       </c>
       <c r="E9">
-        <v>-6.551863544492899</v>
+        <v>-6.552</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -678,16 +678,16 @@
         </is>
       </c>
       <c r="B10">
-        <v>-2.481552991777493</v>
+        <v>-2.482</v>
       </c>
       <c r="C10">
-        <v>1.560652337514508</v>
+        <v>1.561</v>
       </c>
       <c r="D10">
         <v>1669</v>
       </c>
       <c r="E10">
-        <v>-1.590074183805477</v>
+        <v>-1.59</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -712,16 +712,16 @@
         </is>
       </c>
       <c r="B11">
-        <v>-0.9448593487129923</v>
+        <v>-0.945</v>
       </c>
       <c r="C11">
-        <v>0.1185668666661877</v>
+        <v>0.119</v>
       </c>
       <c r="D11">
         <v>1669</v>
       </c>
       <c r="E11">
-        <v>-7.968999900901005</v>
+        <v>-7.969</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -746,16 +746,16 @@
         </is>
       </c>
       <c r="B12">
-        <v>-1.010154017463127</v>
+        <v>-1.01</v>
       </c>
       <c r="C12">
-        <v>0.2868565345721258</v>
+        <v>0.287</v>
       </c>
       <c r="D12">
         <v>1669</v>
       </c>
       <c r="E12">
-        <v>-3.521460715440454</v>
+        <v>-3.521</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -780,16 +780,16 @@
         </is>
       </c>
       <c r="B13">
-        <v>-0.06529466875013512</v>
+        <v>-0.065</v>
       </c>
       <c r="C13">
-        <v>0.2878298192163714</v>
+        <v>0.288</v>
       </c>
       <c r="D13">
         <v>1669</v>
       </c>
       <c r="E13">
-        <v>-0.2268516477128831</v>
+        <v>-0.227</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -814,16 +814,16 @@
         </is>
       </c>
       <c r="B14">
-        <v>-0.5889609891895577</v>
+        <v>-0.589</v>
       </c>
       <c r="C14">
-        <v>0.1916663415973831</v>
+        <v>0.192</v>
       </c>
       <c r="D14">
         <v>1669</v>
       </c>
       <c r="E14">
-        <v>-3.072845155185031</v>
+        <v>-3.073</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -848,16 +848,16 @@
         </is>
       </c>
       <c r="B15">
-        <v>-0.7249886303209311</v>
+        <v>-0.725</v>
       </c>
       <c r="C15">
-        <v>0.4637108501781952</v>
+        <v>0.464</v>
       </c>
       <c r="D15">
         <v>1669</v>
       </c>
       <c r="E15">
-        <v>-1.56344978782</v>
+        <v>-1.563</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -882,16 +882,16 @@
         </is>
       </c>
       <c r="B16">
-        <v>-0.1360276411313733</v>
+        <v>-0.136</v>
       </c>
       <c r="C16">
-        <v>0.4652841894452324</v>
+        <v>0.465</v>
       </c>
       <c r="D16">
         <v>1669</v>
       </c>
       <c r="E16">
-        <v>-0.2923538865431078</v>
+        <v>-0.292</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -916,16 +916,16 @@
         </is>
       </c>
       <c r="B17">
-        <v>-1.250862134081518</v>
+        <v>-1.251</v>
       </c>
       <c r="C17">
-        <v>0.4174189830227573</v>
+        <v>0.417</v>
       </c>
       <c r="D17">
         <v>1669</v>
       </c>
       <c r="E17">
-        <v>-2.996658477348939</v>
+        <v>-2.997</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -950,16 +950,16 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.7417892559774648</v>
+        <v>0.742</v>
       </c>
       <c r="C18">
-        <v>1.009888903209718</v>
+        <v>1.01</v>
       </c>
       <c r="D18">
         <v>1669</v>
       </c>
       <c r="E18">
-        <v>0.7345256033805746</v>
+        <v>0.735</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -984,16 +984,16 @@
         </is>
       </c>
       <c r="B19">
-        <v>1.992651390058983</v>
+        <v>1.993</v>
       </c>
       <c r="C19">
-        <v>1.013315387334802</v>
+        <v>1.013</v>
       </c>
       <c r="D19">
         <v>1669</v>
       </c>
       <c r="E19">
-        <v>1.966467118692441</v>
+        <v>1.966</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1018,16 +1018,16 @@
         </is>
       </c>
       <c r="B20">
-        <v>-6.482947122466972</v>
+        <v>-6.483</v>
       </c>
       <c r="C20">
-        <v>0.5553707430451689</v>
+        <v>0.555</v>
       </c>
       <c r="D20">
         <v>1669</v>
       </c>
       <c r="E20">
-        <v>-11.67318805257933</v>
+        <v>-11.673</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="B21">
-        <v>-7.966146507491916</v>
+        <v>-7.966</v>
       </c>
       <c r="C21">
-        <v>1.343644571473823</v>
+        <v>1.344</v>
       </c>
       <c r="D21">
         <v>1669</v>
       </c>
       <c r="E21">
-        <v>-5.928760236610767</v>
+        <v>-5.929</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1086,16 +1086,16 @@
         </is>
       </c>
       <c r="B22">
-        <v>-1.483199385024944</v>
+        <v>-1.483</v>
       </c>
       <c r="C22">
-        <v>1.34820346580297</v>
+        <v>1.348</v>
       </c>
       <c r="D22">
         <v>1669</v>
       </c>
       <c r="E22">
-        <v>-1.10013022711047</v>
+        <v>-1.1</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1120,16 +1120,16 @@
         </is>
       </c>
       <c r="B23">
-        <v>-1.563237305416217</v>
+        <v>-1.563</v>
       </c>
       <c r="C23">
-        <v>0.5890511945642841</v>
+        <v>0.589</v>
       </c>
       <c r="D23">
         <v>1669</v>
       </c>
       <c r="E23">
-        <v>-2.653822485790101</v>
+        <v>-2.654</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1154,16 +1154,16 @@
         </is>
       </c>
       <c r="B24">
-        <v>-5.639602962653083</v>
+        <v>-5.64</v>
       </c>
       <c r="C24">
-        <v>1.425129879108701</v>
+        <v>1.425</v>
       </c>
       <c r="D24">
         <v>1669</v>
       </c>
       <c r="E24">
-        <v>-3.957255437083517</v>
+        <v>-3.957</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1188,16 +1188,16 @@
         </is>
       </c>
       <c r="B25">
-        <v>-4.076365657236867</v>
+        <v>-4.076</v>
       </c>
       <c r="C25">
-        <v>1.429965247525395</v>
+        <v>1.43</v>
       </c>
       <c r="D25">
         <v>1669</v>
       </c>
       <c r="E25">
-        <v>-2.85067463303123</v>
+        <v>-2.851</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1222,16 +1222,16 @@
         </is>
       </c>
       <c r="B26">
-        <v>-0.8181144745052047</v>
+        <v>-0.8179999999999999</v>
       </c>
       <c r="C26">
-        <v>0.2918412652427201</v>
+        <v>0.292</v>
       </c>
       <c r="D26">
         <v>1669</v>
       </c>
       <c r="E26">
-        <v>-2.80328579930186</v>
+        <v>-2.803</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1256,16 +1256,16 @@
         </is>
       </c>
       <c r="B27">
-        <v>-2.019773318270061</v>
+        <v>-2.02</v>
       </c>
       <c r="C27">
-        <v>0.7060705604067814</v>
+        <v>0.706</v>
       </c>
       <c r="D27">
         <v>1669</v>
       </c>
       <c r="E27">
-        <v>-2.860582824904113</v>
+        <v>-2.861</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1290,16 +1290,16 @@
         </is>
       </c>
       <c r="B28">
-        <v>-1.201658843764856</v>
+        <v>-1.202</v>
       </c>
       <c r="C28">
-        <v>0.7084662096299126</v>
+        <v>0.708</v>
       </c>
       <c r="D28">
         <v>1669</v>
       </c>
       <c r="E28">
-        <v>-1.696141364868448</v>
+        <v>-1.696</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>

</xml_diff>